<commit_message>
đã in phiếu(chưa lên giao diện)
</commit_message>
<xml_diff>
--- a/api/List of candidates/students.xlsx
+++ b/api/List of candidates/students.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhng\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edu\Python\StudentID_FaceVerification\student-id-face-matching\api\List of candidates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDA8EC6-7F34-4D89-B5A0-50C3C86B0C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54381338-D43A-434A-AFC3-C466797437E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3097" yWindow="3097" windowWidth="19563" windowHeight="10162" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Họ Tên</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Trần Thị Thanh</t>
+  </si>
+  <si>
+    <t>Đặng Ngọc Anh</t>
+  </si>
+  <si>
+    <t>Thái Văn Tuấn</t>
   </si>
 </sst>
 </file>
@@ -465,20 +471,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -500,7 +506,7 @@
         <v>912345001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -511,7 +517,7 @@
         <v>912345002</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -522,7 +528,7 @@
         <v>912345003</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -533,7 +539,7 @@
         <v>912345004</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -544,7 +550,7 @@
         <v>912345005</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -555,7 +561,7 @@
         <v>912345006</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -566,7 +572,7 @@
         <v>912345007</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -577,7 +583,7 @@
         <v>912345008</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -588,7 +594,7 @@
         <v>912345009</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -599,7 +605,7 @@
         <v>912345010</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -610,7 +616,7 @@
         <v>912345011</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -621,7 +627,7 @@
         <v>912345012</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -632,7 +638,7 @@
         <v>912345013</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -643,7 +649,7 @@
         <v>912345014</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -654,7 +660,7 @@
         <v>912345015</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -665,7 +671,7 @@
         <v>912345016</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -676,7 +682,7 @@
         <v>912345017</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -687,7 +693,7 @@
         <v>912345018</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -698,7 +704,7 @@
         <v>912345019</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -707,6 +713,28 @@
       </c>
       <c r="C21">
         <v>912345020</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>215748020110333</v>
+      </c>
+      <c r="C22">
+        <v>344483272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>215748020110086</v>
+      </c>
+      <c r="C23">
+        <v>987654321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>